<commit_message>
Second scenario added - Dataset has changed a bit - A little refactor
</commit_message>
<xml_diff>
--- a/apple_dataset.xlsx
+++ b/apple_dataset.xlsx
@@ -1005,7 +1005,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1040,6 +1040,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="59" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2339,11 +2342,13 @@
         <v>46</v>
       </c>
       <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="12">
+      <c r="I3" s="12">
+        <v>7</v>
+      </c>
+      <c r="J3" s="13">
         <v>38.25424</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="13">
         <v>-85.75941</v>
       </c>
       <c r="L3" t="s" s="10">
@@ -2355,13 +2360,13 @@
       <c r="N3" t="s" s="10">
         <v>49</v>
       </c>
-      <c r="O3" s="13">
+      <c r="O3" s="14">
         <v>1836</v>
       </c>
-      <c r="P3" s="13">
+      <c r="P3" s="14">
         <v>967</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="Q3" s="14">
         <v>293</v>
       </c>
       <c r="R3" t="s" s="10">
@@ -2411,7 +2416,9 @@
         <v>60</v>
       </c>
       <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="I4" s="12">
+        <v>10</v>
+      </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
@@ -2419,13 +2426,13 @@
       <c r="N4" t="s" s="10">
         <v>61</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="14">
         <v>27</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="14">
         <v>3</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="Q4" s="14">
         <v>38</v>
       </c>
       <c r="R4" t="s" s="10">
@@ -2473,7 +2480,9 @@
         <v>68</v>
       </c>
       <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="I5" s="12">
+        <v>3</v>
+      </c>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
@@ -2481,13 +2490,13 @@
       <c r="N5" t="s" s="10">
         <v>69</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="14">
         <v>24</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="14">
         <v>2</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="14">
         <v>38</v>
       </c>
       <c r="R5" t="s" s="10">
@@ -2535,7 +2544,9 @@
         <v>76</v>
       </c>
       <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="I6" s="12">
+        <v>1</v>
+      </c>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
@@ -2543,13 +2554,13 @@
       <c r="N6" t="s" s="10">
         <v>77</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="14">
         <v>1602</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="14">
         <v>2029</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="14">
         <v>108</v>
       </c>
       <c r="R6" t="s" s="10">
@@ -2592,10 +2603,12 @@
       <c r="G7" t="s" s="10">
         <v>84</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="14">
         <v>1</v>
       </c>
-      <c r="I7" s="11"/>
+      <c r="I7" s="12">
+        <v>4</v>
+      </c>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
@@ -2603,13 +2616,13 @@
       <c r="N7" t="s" s="10">
         <v>85</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="14">
         <v>105</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="14">
         <v>330</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="Q7" s="14">
         <v>17</v>
       </c>
       <c r="R7" t="s" s="10">
@@ -2655,7 +2668,9 @@
         <v>93</v>
       </c>
       <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="I8" s="12">
+        <v>3</v>
+      </c>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
@@ -2663,13 +2678,13 @@
       <c r="N8" t="s" s="10">
         <v>94</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="14">
         <v>2768</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="14">
         <v>2762</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q8" s="14">
         <v>279</v>
       </c>
       <c r="R8" t="s" s="10">
@@ -2715,11 +2730,13 @@
         <v>102</v>
       </c>
       <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12">
+      <c r="I9" s="12">
+        <v>11</v>
+      </c>
+      <c r="J9" s="13">
         <v>44.26193</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="13">
         <v>-88.41538</v>
       </c>
       <c r="L9" t="s" s="10">
@@ -2731,13 +2748,13 @@
       <c r="N9" t="s" s="10">
         <v>104</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="14">
         <v>626</v>
       </c>
-      <c r="P9" s="13">
+      <c r="P9" s="14">
         <v>2001</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="Q9" s="14">
         <v>22</v>
       </c>
       <c r="R9" t="s" s="10">
@@ -2783,11 +2800,13 @@
         <v>111</v>
       </c>
       <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12">
+      <c r="I10" s="12">
+        <v>2</v>
+      </c>
+      <c r="J10" s="13">
         <v>45.41117</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="13">
         <v>-75.69812</v>
       </c>
       <c r="L10" t="s" s="10">
@@ -2799,13 +2818,13 @@
       <c r="N10" t="s" s="10">
         <v>114</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="14">
         <v>1503</v>
       </c>
-      <c r="P10" s="13">
+      <c r="P10" s="14">
         <v>256</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="Q10" s="14">
         <v>75</v>
       </c>
       <c r="R10" t="s" s="10">

</xml_diff>